<commit_message>
PAM, TOP2VEC, NEWPAPERS, REFINEMENT, TARGETS
</commit_message>
<xml_diff>
--- a/Project_python/out/matrix_classification_abstract.xlsx
+++ b/Project_python/out/matrix_classification_abstract.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[0.07248387817756036]</t>
+          <t>[0.023536610578377744]</t>
         </is>
       </c>
       <c r="F2" t="b">
@@ -517,7 +517,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[0.05015196694862146]</t>
+          <t>[0.04945740746029779]</t>
         </is>
       </c>
       <c r="F3" t="b">
@@ -548,7 +548,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[0.019780000438122922, 0.01918424360331902]</t>
+          <t>[0.01741634835906335, 0.016454188862395067]</t>
         </is>
       </c>
       <c r="F4" t="b">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[10]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -579,7 +579,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[0.05918929996333007]</t>
+          <t>[0.08209356049895129]</t>
         </is>
       </c>
       <c r="F5" t="b">
@@ -610,7 +610,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[0.05392743394541637]</t>
+          <t>[0.055635642885898846]</t>
         </is>
       </c>
       <c r="F6" t="b">
@@ -631,7 +631,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[0.03109436233987639]</t>
+          <t>[0.027005319549134987]</t>
         </is>
       </c>
       <c r="F7" t="b">
@@ -672,7 +672,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[0.07428089188932807]</t>
+          <t>[0.07080912413786222]</t>
         </is>
       </c>
       <c r="F8" t="b">
@@ -703,7 +703,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[0.08619368202318715]</t>
+          <t>[0.0742423590133723]</t>
         </is>
       </c>
       <c r="F9" t="b">
@@ -734,7 +734,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[0.04790717434977627]</t>
+          <t>[0.03823278672278228]</t>
         </is>
       </c>
       <c r="F10" t="b">
@@ -765,7 +765,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[0.09327020809922026]</t>
+          <t>[0.08626336155443307]</t>
         </is>
       </c>
       <c r="F11" t="b">
@@ -796,7 +796,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[0.03339494036058322]</t>
+          <t>[0.03088291638730878]</t>
         </is>
       </c>
       <c r="F12" t="b">
@@ -827,7 +827,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[0.08946038595661406]</t>
+          <t>[0.04930673121686159]</t>
         </is>
       </c>
       <c r="F13" t="b">
@@ -858,7 +858,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[0.05500096450734547]</t>
+          <t>[0.04722684913617175]</t>
         </is>
       </c>
       <c r="F14" t="b">
@@ -879,7 +879,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[17, 3]</t>
+          <t>[3, 12]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[0.02104694326286252, 0.018579265093469934]</t>
+          <t>[0.014231877735163479, 0.011824962225551575]</t>
         </is>
       </c>
       <c r="F15" t="b">
@@ -920,7 +920,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[0.07601410173296694]</t>
+          <t>[0.06588499828846661]</t>
         </is>
       </c>
       <c r="F16" t="b">
@@ -951,7 +951,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[0.0472435756299213]</t>
+          <t>[0.04671551399509548]</t>
         </is>
       </c>
       <c r="F17" t="b">
@@ -982,7 +982,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[0.027117125456643503]</t>
+          <t>[0.024710214004333767]</t>
         </is>
       </c>
       <c r="F18" t="b">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[0.02918083447732448]</t>
+          <t>[0.029271213044384292]</t>
         </is>
       </c>
       <c r="F19" t="b">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[17, 14]</t>
+          <t>[12, 14]</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[0.06992378212375175, 0.023454763424133006]</t>
+          <t>[0.030057252076297943, 0.028240373921226178]</t>
         </is>
       </c>
       <c r="F20" t="b">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[0.013855962587697687]</t>
+          <t>[0.013208651213482294]</t>
         </is>
       </c>
       <c r="F21" t="b">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[0.019531331716401597]</t>
+          <t>[0.019543953671839937]</t>
         </is>
       </c>
       <c r="F22" t="b">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[0.031834934562794105]</t>
+          <t>[0.019866816154563472]</t>
         </is>
       </c>
       <c r="F23" t="b">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>[0.08372127049714377]</t>
+          <t>[0.022864741843182466]</t>
         </is>
       </c>
       <c r="F24" t="b">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[0.019467018526012396]</t>
+          <t>[0.0217358841068465]</t>
         </is>
       </c>
       <c r="F25" t="b">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[8, 12]</t>
+          <t>[12, 8]</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[0.03218216081004698, 0.02915358929649803]</t>
+          <t>[0.026667865951857883, 0.018079812237319245]</t>
         </is>
       </c>
       <c r="F26" t="b">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[0.02718417150813917, 0.015186781967513486]</t>
+          <t>[0.017856235437780737, 0.014601828622635663]</t>
         </is>
       </c>
       <c r="F27" t="b">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[0.03978018999172289]</t>
+          <t>[0.03440730387059832]</t>
         </is>
       </c>
       <c r="F28" t="b">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[0.14018887031022773]</t>
+          <t>[0.12201920511257586]</t>
         </is>
       </c>
       <c r="F29" t="b">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>[16]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[0.016538872717160067]</t>
+          <t>[0.015224711109669421]</t>
         </is>
       </c>
       <c r="F30" t="b">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>[17, 16]</t>
+          <t>[4, 12]</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[0.04877356363923416, 0.02192259838455848]</t>
+          <t>[0.022983111225864994, 0.021128104959110414]</t>
         </is>
       </c>
       <c r="F31" t="b">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[0.037175995183436054]</t>
+          <t>[0.041960500206209464]</t>
         </is>
       </c>
       <c r="F32" t="b">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[0.02291380439360097]</t>
+          <t>[0.023164318946890947]</t>
         </is>
       </c>
       <c r="F33" t="b">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[0.06969044114019725]</t>
+          <t>[0.04097486955322327]</t>
         </is>
       </c>
       <c r="F34" t="b">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[0.06197990423377508]</t>
+          <t>[0.05367653833454907]</t>
         </is>
       </c>
       <c r="F35" t="b">
@@ -1530,24 +1530,24 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>[3]</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>[3]</t>
-        </is>
-      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>[0.030356137268124188]</t>
+          <t>[0.026878418818932777]</t>
         </is>
       </c>
       <c r="F36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[0.037975793044350836]</t>
+          <t>[0.03352325313079837]</t>
         </is>
       </c>
       <c r="F37" t="b">
@@ -1602,7 +1602,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[0.018329391270429006]</t>
+          <t>[0.015247649546653039]</t>
         </is>
       </c>
       <c r="F38" t="b">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[0.028116488719195837]</t>
+          <t>[0.02311437376307062]</t>
         </is>
       </c>
       <c r="F39" t="b">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[0.024505151751712872]</t>
+          <t>[0.01995616305638218]</t>
         </is>
       </c>
       <c r="F40" t="b">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1695,14 +1695,14 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[0.05108854225905183]</t>
+          <t>[0.02780445063449169]</t>
         </is>
       </c>
       <c r="F41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[0.029984032994170705]</t>
+          <t>[0.027771491637418225]</t>
         </is>
       </c>
       <c r="F42" t="b">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[0.05033218695568226]</t>
+          <t>[0.03932267105369159]</t>
         </is>
       </c>
       <c r="F43" t="b">
@@ -1778,24 +1778,24 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>[2]</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>[3]</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>[3]</t>
-        </is>
-      </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[0.021731702212204093]</t>
+          <t>[0.01851150147496339]</t>
         </is>
       </c>
       <c r="F44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[5]</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[0.055731224169965406]</t>
+          <t>[0.014070830323981272]</t>
         </is>
       </c>
       <c r="F45" t="b">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[0.022057430661825528, 0.016633683227472537]</t>
+          <t>[0.019392280452125737, 0.0157897259860229]</t>
         </is>
       </c>
       <c r="F46" t="b">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[0.018296854426119166]</t>
+          <t>[0.018856267397858183]</t>
         </is>
       </c>
       <c r="F47" t="b">
@@ -1912,7 +1912,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[0.017256246577607284, 0.013093623916175013]</t>
+          <t>[0.01653772115384623, 0.013234910023625533]</t>
         </is>
       </c>
       <c r="F48" t="b">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1943,14 +1943,14 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[0.025672675712008083]</t>
+          <t>[0.012144709094922814]</t>
         </is>
       </c>
       <c r="F49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[0.05331004272593318]</t>
+          <t>[0.055623751836235705]</t>
         </is>
       </c>
       <c r="F50" t="b">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[0.04234454683740382]</t>
+          <t>[0.03203874830156629]</t>
         </is>
       </c>
       <c r="F51" t="b">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.1119670357645509]</t>
+          <t>[0.1259522414968788]</t>
         </is>
       </c>
       <c r="F52" t="b">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[0.03805312603675271]</t>
+          <t>[0.042662247426591506]</t>
         </is>
       </c>
       <c r="F53" t="b">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2098,14 +2098,14 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>[0.06704426756312985]</t>
+          <t>[0.041825346764005386]</t>
         </is>
       </c>
       <c r="F54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[0.036895891435610395]</t>
+          <t>[0.039538472823479304]</t>
         </is>
       </c>
       <c r="F55" t="b">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2160,14 +2160,14 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>[0.044936738637248154]</t>
+          <t>[0.025093806992813595]</t>
         </is>
       </c>
       <c r="F56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>[0.04245497335698071]</t>
+          <t>[0.023617243390953876]</t>
         </is>
       </c>
       <c r="F57" t="b">
@@ -2222,7 +2222,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[0.026730747509507734]</t>
+          <t>[0.028299377081935678]</t>
         </is>
       </c>
       <c r="F58" t="b">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>[0.035126694824446844]</t>
+          <t>[0.031191442816342153]</t>
         </is>
       </c>
       <c r="F59" t="b">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>[0.019570329689957918]</t>
+          <t>[0.019643818445183203]</t>
         </is>
       </c>
       <c r="F60" t="b">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[0.15784874064453686]</t>
+          <t>[0.11791829813455898]</t>
         </is>
       </c>
       <c r="F61" t="b">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[0.05771884633174453]</t>
+          <t>[0.0492863470657211]</t>
         </is>
       </c>
       <c r="F62" t="b">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>[0.03866188725808945]</t>
+          <t>[0.03225621104676025]</t>
         </is>
       </c>
       <c r="F63" t="b">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[0.049729783162117056]</t>
+          <t>[0.040117852847178725]</t>
         </is>
       </c>
       <c r="F64" t="b">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>[0.07191542556750795]</t>
+          <t>[0.062276700229172595]</t>
         </is>
       </c>
       <c r="F65" t="b">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2470,7 +2470,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>[0.08889438017643916]</t>
+          <t>[0.026360732153291534]</t>
         </is>
       </c>
       <c r="F66" t="b">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[0.018767993080666796]</t>
+          <t>[0.010039502982408223]</t>
         </is>
       </c>
       <c r="F67" t="b">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>[0.01818672616223885]</t>
+          <t>[0.01828612633272732]</t>
         </is>
       </c>
       <c r="F68" t="b">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>[0.04671236657144164]</t>
+          <t>[0.027025164652267314]</t>
         </is>
       </c>
       <c r="F69" t="b">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.07046660578008312]</t>
+          <t>[0.07028117101515562]</t>
         </is>
       </c>
       <c r="F70" t="b">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[6]</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2625,14 +2625,14 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>[0.06078702681963475]</t>
+          <t>[0.03524868034040787]</t>
         </is>
       </c>
       <c r="F71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>[0.06496534076006102]</t>
+          <t>[0.0647253762082359]</t>
         </is>
       </c>
       <c r="F72" t="b">
@@ -2677,7 +2677,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>[15, 17]</t>
+          <t>[15, 13]</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[0.032755735162353035, 0.027328479111176838]</t>
+          <t>[0.03312122588361357, 0.021366108757078856]</t>
         </is>
       </c>
       <c r="F73" t="b">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>[0.1588609502940752]</t>
+          <t>[0.1429906240368885]</t>
         </is>
       </c>
       <c r="F74" t="b">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[5]</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[0.02305073096600642]</t>
+          <t>[0.020565434116998495]</t>
         </is>
       </c>
       <c r="F75" t="b">
@@ -2770,7 +2770,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2811,7 +2811,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>[0.05003878256087149]</t>
+          <t>[0.01986086174169872]</t>
         </is>
       </c>
       <c r="F77" t="b">
@@ -2832,24 +2832,24 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
+          <t>[9]</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
           <t>[8]</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>[8]</t>
-        </is>
-      </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>[0.027755340250391534]</t>
+          <t>[0.02451186508899541]</t>
         </is>
       </c>
       <c r="F78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.044556159617890646, 0.015922539569005634]</t>
+          <t>[0.02729181085789471, 0.013550026463560138]</t>
         </is>
       </c>
       <c r="F79" t="b">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>[0.0737630750624083]</t>
+          <t>[0.026658506359046846]</t>
         </is>
       </c>
       <c r="F80" t="b">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2935,7 +2935,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>[0.06191107494649853]</t>
+          <t>[0.011373484120333684]</t>
         </is>
       </c>
       <c r="F81" t="b">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>[0.05024428289114881, 0.0187391079826208]</t>
+          <t>[0.028677689808275238, 0.020570973119316455]</t>
         </is>
       </c>
       <c r="F82" t="b">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>[0.04753123628958015]</t>
+          <t>[0.03525105907520156]</t>
         </is>
       </c>
       <c r="F83" t="b">
@@ -3018,7 +3018,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>[0.01372697842394908]</t>
+          <t>[0.01564550248275143]</t>
         </is>
       </c>
       <c r="F84" t="b">
@@ -3059,7 +3059,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>[0.04159161696574442]</t>
+          <t>[0.037891235218253105]</t>
         </is>
       </c>
       <c r="F85" t="b">
@@ -3080,7 +3080,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3090,14 +3090,14 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>[0.02405182686131338]</t>
+          <t>[0.01787218664942626]</t>
         </is>
       </c>
       <c r="F86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>[0.010314084597107216, 0.010134773419939012]</t>
+          <t>[0.009671399604483752, 0.008001429128164466]</t>
         </is>
       </c>
       <c r="F87" t="b">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>[11, 17]</t>
+          <t>[11, 9]</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3152,11 +3152,11 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>[0.16843231446704962, 0.05694230963662006]</t>
+          <t>[0.13485387620366296, 0.023004045981285658]</t>
         </is>
       </c>
       <c r="F88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88" t="b">
         <v>1</v>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>[6, 17]</t>
+          <t>[6, 11]</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3183,14 +3183,14 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>[0.13852073915622284, 0.07240714571538008]</t>
+          <t>[0.12192448028248166, 0.03659580090317025]</t>
         </is>
       </c>
       <c r="F89" t="b">
         <v>0</v>
       </c>
       <c r="G89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -3214,7 +3214,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>[0.03973545644065789, 0.023506261289329405]</t>
+          <t>[0.03472494291837562, 0.020178443002616054]</t>
         </is>
       </c>
       <c r="F90" t="b">
@@ -3235,7 +3235,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3245,14 +3245,14 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>[0.03848244798471342]</t>
+          <t>[0.029476559692745614]</t>
         </is>
       </c>
       <c r="F91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>[0.024942367162678274]</t>
+          <t>[0.025684077013547385]</t>
         </is>
       </c>
       <c r="F92" t="b">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>[0.03191993058553606]</t>
+          <t>[0.01927843887099886]</t>
         </is>
       </c>
       <c r="F93" t="b">
@@ -3328,7 +3328,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[5]</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>[0.03466991551884797]</t>
+          <t>[0.025178644839921015]</t>
         </is>
       </c>
       <c r="F94" t="b">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>[0.020081367214719578]</t>
+          <t>[0.01812798891134787]</t>
         </is>
       </c>
       <c r="F95" t="b">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>[0.13591627914793644]</t>
+          <t>[0.1214549299649357]</t>
         </is>
       </c>
       <c r="F96" t="b">
@@ -3431,7 +3431,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>[0.030577128756076582]</t>
+          <t>[0.020639683043695928]</t>
         </is>
       </c>
       <c r="F97" t="b">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>[0.05217582205625303]</t>
+          <t>[0.04696509180762478]</t>
         </is>
       </c>
       <c r="F98" t="b">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>[0.24627437794688203]</t>
+          <t>[0.19867664263780146]</t>
         </is>
       </c>
       <c r="F99" t="b">
@@ -3514,7 +3514,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3545,7 +3545,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>[12]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>[0.015271189164547519]</t>
+          <t>[0.011700001548376544]</t>
         </is>
       </c>
       <c r="F101" t="b">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>[0.028690662500219587]</t>
+          <t>[0.018472659472500572]</t>
         </is>
       </c>
       <c r="F102" t="b">
@@ -3617,7 +3617,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>[0.06945704150668786]</t>
+          <t>[0.06219429371157387]</t>
         </is>
       </c>
       <c r="F103" t="b">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>[0.04263184999082741]</t>
+          <t>[0.03186240427574148]</t>
         </is>
       </c>
       <c r="F104" t="b">
@@ -3679,7 +3679,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>[0.07776334760057618]</t>
+          <t>[0.048769451091456695]</t>
         </is>
       </c>
       <c r="F105" t="b">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>[0.1440598861608188]</t>
+          <t>[0.13973753211116702]</t>
         </is>
       </c>
       <c r="F106" t="b">
@@ -3731,7 +3731,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>[8]</t>
+          <t>[3]</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>[0.0193430354920434]</t>
+          <t>[0.013328806688617236]</t>
         </is>
       </c>
       <c r="F107" t="b">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>[0.020182694500192767]</t>
+          <t>[0.017814070664961892]</t>
         </is>
       </c>
       <c r="F108" t="b">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[4]</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>[0.0295869130956023]</t>
+          <t>[0.02518331315736751]</t>
         </is>
       </c>
       <c r="F109" t="b">
@@ -3834,7 +3834,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>[0.2305004889043337]</t>
+          <t>[0.25059363080278724]</t>
         </is>
       </c>
       <c r="F110" t="b">
@@ -3855,7 +3855,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[11]</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>[0.030582574912143425]</t>
+          <t>[0.006603049022242371]</t>
         </is>
       </c>
       <c r="F111" t="b">
@@ -3896,7 +3896,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>[0.15233855082507955]</t>
+          <t>[0.12269121035917183]</t>
         </is>
       </c>
       <c r="F112" t="b">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3958,7 +3958,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>[0.030914732217022498]</t>
+          <t>[0.01660350998620207]</t>
         </is>
       </c>
       <c r="F114" t="b">
@@ -3979,7 +3979,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>[0.07807832344937776]</t>
+          <t>[0.08437592510379595]</t>
         </is>
       </c>
       <c r="F116" t="b">
@@ -4051,7 +4051,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>[0.07134831075017076]</t>
+          <t>[0.0719803487290318]</t>
         </is>
       </c>
       <c r="F117" t="b">
@@ -4082,7 +4082,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>[0.10475243819697154]</t>
+          <t>[0.1070993383593381]</t>
         </is>
       </c>
       <c r="F118" t="b">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>[0.026845831842092605]</t>
+          <t>[0.02594710001961587]</t>
         </is>
       </c>
       <c r="F120" t="b">
@@ -4175,7 +4175,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>[0.08586998128621919]</t>
+          <t>[0.07099534397421887]</t>
         </is>
       </c>
       <c r="F121" t="b">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>[0.107138753027404]</t>
+          <t>[0.11587333532338244]</t>
         </is>
       </c>
       <c r="F122" t="b">
@@ -4237,7 +4237,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>[0.07621938294359022]</t>
+          <t>[0.08621974991519225]</t>
         </is>
       </c>
       <c r="F123" t="b">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>[0.04868411972455289]</t>
+          <t>[0.04507826099362961]</t>
         </is>
       </c>
       <c r="F124" t="b">
@@ -4299,7 +4299,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>[0.04022561621788317]</t>
+          <t>[0.04424842157061594]</t>
         </is>
       </c>
       <c r="F125" t="b">
@@ -4330,7 +4330,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>[0.018744228785134952]</t>
+          <t>[0.021629960479859305]</t>
         </is>
       </c>
       <c r="F126" t="b">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>[0.09094153040133114]</t>
+          <t>[0.08020163404158934]</t>
         </is>
       </c>
       <c r="F127" t="b">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>[0.0964101443338521]</t>
+          <t>[0.1038212354531301]</t>
         </is>
       </c>
       <c r="F128" t="b">
@@ -4423,7 +4423,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>[0.15044485337751837]</t>
+          <t>[0.1471874720925365]</t>
         </is>
       </c>
       <c r="F129" t="b">
@@ -4454,7 +4454,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>[0.06537121915707446]</t>
+          <t>[0.06207815271872887]</t>
         </is>
       </c>
       <c r="F130" t="b">
@@ -4475,7 +4475,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[15]</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -4485,14 +4485,14 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>[0.047098867921476446]</t>
+          <t>[0.031189853286459825]</t>
         </is>
       </c>
       <c r="F131" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G131" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -4516,7 +4516,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>[0.09446468091384595]</t>
+          <t>[0.08221003238258262]</t>
         </is>
       </c>
       <c r="F132" t="b">
@@ -4547,7 +4547,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>[0.09382953718987526]</t>
+          <t>[0.08159725862111847]</t>
         </is>
       </c>
       <c r="F133" t="b">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4578,14 +4578,14 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>[0.02064562235660573]</t>
+          <t>[0.019380874498584437]</t>
         </is>
       </c>
       <c r="F134" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G134" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -4599,7 +4599,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4609,14 +4609,14 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>[0.036852391667815745]</t>
+          <t>[0.01892183674140469]</t>
         </is>
       </c>
       <c r="F135" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G135" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
@@ -4640,7 +4640,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>[0.03253783236513268]</t>
+          <t>[0.027290747906282452]</t>
         </is>
       </c>
       <c r="F136" t="b">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>[1]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4671,14 +4671,14 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>[0.037838002790226026]</t>
+          <t>[0.03377110033672191]</t>
         </is>
       </c>
       <c r="F137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -4692,7 +4692,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4702,7 +4702,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>[0.03407104258737317]</t>
+          <t>[0.028705459141617887]</t>
         </is>
       </c>
       <c r="F138" t="b">
@@ -4723,7 +4723,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>[17]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>[0.08361348535987788]</t>
+          <t>[0.015859120804784233]</t>
         </is>
       </c>
       <c r="F139" t="b">
@@ -4764,7 +4764,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>[0.027144768596056128]</t>
+          <t>[0.021597290710901995]</t>
         </is>
       </c>
       <c r="F140" t="b">
@@ -4795,7 +4795,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>[0.009876631953536313]</t>
+          <t>[0.00882603834948155]</t>
         </is>
       </c>
       <c r="F141" t="b">

</xml_diff>